<commit_message>
completed add on order for personal purchase
</commit_message>
<xml_diff>
--- a/NewArrivals/credData.xlsx
+++ b/NewArrivals/credData.xlsx
@@ -78,13 +78,13 @@
     <t>CWpass</t>
   </si>
   <si>
-    <t>https://test14.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test14.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test14.cliotest.com/warehouse/control/main</t>
+    <t>https://test17.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test17.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test17.cliotest.com/warehouse/control/main</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated cred for pushOfbiz
</commit_message>
<xml_diff>
--- a/NewArrivals/credData.xlsx
+++ b/NewArrivals/credData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>400000002</t>
   </si>
@@ -48,12 +48,6 @@
     <t>BOpass</t>
   </si>
   <si>
-    <t>sshinde</t>
-  </si>
-  <si>
-    <t>C@bi$ush5</t>
-  </si>
-  <si>
     <t>CCuser</t>
   </si>
   <si>
@@ -85,6 +79,9 @@
   </si>
   <si>
     <t>https://test17.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
@@ -524,7 +521,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -557,27 +554,27 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
       <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
       <c r="L1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -589,25 +586,25 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1234</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
         <v>1</v>
@@ -616,7 +613,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" display="C@bi$ush5"/>
     <hyperlink ref="G2" r:id="rId2"/>
     <hyperlink ref="J2" r:id="rId3"/>
     <hyperlink ref="A2" r:id="rId4"/>

</xml_diff>

<commit_message>
dynamic object creation (passing dynammic xpath) for rsOrderHistoryConfirm
</commit_message>
<xml_diff>
--- a/NewArrivals/credData.xlsx
+++ b/NewArrivals/credData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation_new\NewArrivals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation\NewArrivals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -99,7 +99,7 @@
     <t>https://test3.cliotest.com/backoffice/control/main</t>
   </si>
   <si>
-    <t>https://mirandakate.cabitest3.com/</t>
+    <t>https://mirandakate.cabitest3.com</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +549,7 @@
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="36.140625" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completed gift card and donation scenarios
</commit_message>
<xml_diff>
--- a/NewArrivals/credData.xlsx
+++ b/NewArrivals/credData.xlsx
@@ -72,12 +72,6 @@
     <t>CWpass</t>
   </si>
   <si>
-    <t>https://test14.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test14.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
     <t>sshinde</t>
   </si>
   <si>
@@ -96,10 +90,16 @@
     <t>RSpass</t>
   </si>
   <si>
-    <t>https://test3.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest3.com</t>
+    <t>https://mirandakate.cabitest4.com</t>
+  </si>
+  <si>
+    <t>https://test4.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test4.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>https://test4.cliotest.com/backoffice/control/main</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -590,18 +590,18 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
       <c r="O1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -613,13 +613,13 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -628,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
@@ -637,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
         <v>1</v>
@@ -652,7 +652,7 @@
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="G2" r:id="rId2" display="https://test17.cliotest.com/cabicentral/control/main"/>
     <hyperlink ref="J2" r:id="rId3" display="https://test17.cliotest.com/warehouse/control/main"/>
-    <hyperlink ref="A2" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId4" display="https://test3.cliotest.com/backoffice/control/main"/>
     <hyperlink ref="M2" r:id="rId5"/>
     <hyperlink ref="N2" r:id="rId6"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Improved retail order for edit order project
</commit_message>
<xml_diff>
--- a/NewArrivals/credData.xlsx
+++ b/NewArrivals/credData.xlsx
@@ -90,16 +90,16 @@
     <t>RSpass</t>
   </si>
   <si>
-    <t>https://test19.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test19.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test19.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabitest19.com</t>
+    <t>https://test21.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test21.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test21.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>https://mirandakate.cabitest21.com</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -651,9 +651,9 @@
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="G2" r:id="rId2" display="https://test17.cliotest.com/cabicentral/control/main"/>
-    <hyperlink ref="J2" r:id="rId3" display="https://test17.cliotest.com/warehouse/control/main"/>
+    <hyperlink ref="J2" r:id="rId3" display="https://test19.cliotest.com/warehouse/control/main"/>
     <hyperlink ref="A2" r:id="rId4" display="https://test4.cliotest.com/backoffice/control/main"/>
-    <hyperlink ref="M2" r:id="rId5"/>
+    <hyperlink ref="M2" r:id="rId5" display="https://mirandakate.cabitest19.com"/>
     <hyperlink ref="N2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>